<commit_message>
[FEAT]:never invest sth u don't konw
Signed-off-by: Luke Lv 吕铮 <lukelv@vastaitech.com>
</commit_message>
<xml_diff>
--- a/000/invest/daily.xlsx
+++ b/000/invest/daily.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\repo_git\dao_loc\DAO\000\invest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D2D71F-5D58-4BD9-BDD5-EA6731BBC96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3754C0-0E2B-4868-9EBF-508518894509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>周一</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -50,6 +50,12 @@
     <t>1、右侧，保持顺势而为。人多的地方，晚点去；人都走，我就进。
 2、沉没成本，一定时限后就不再计入成本。
 3、运势命，三者缺一不可。乘运而起，顺势而为，命皆有数。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、人多的地方我不去
+2、沉没成本，及时止损
+3、走同一种道路</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -115,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -125,6 +131,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,7 +418,7 @@
   <dimension ref="A1:AG55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -503,11 +512,13 @@
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
     </row>
-    <row r="3" spans="1:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>

</xml_diff>